<commit_message>
Formatting of Change Log.xlsx
</commit_message>
<xml_diff>
--- a/Documents/Change Log.xlsx
+++ b/Documents/Change Log.xlsx
@@ -104,9 +104,6 @@
     <t>Included Shopping Module into scope</t>
   </si>
   <si>
-    <t>Expound on the e-commerce aspect of the site, provide a platform for aspiring game providers resources to start their game designs</t>
-  </si>
-  <si>
     <t>Extend Game Server to a separate server</t>
   </si>
   <si>
@@ -138,6 +135,10 @@
   </si>
   <si>
     <t>27.12.17</t>
+  </si>
+  <si>
+    <t>Expound on the 
+e-commerce aspect of the site, provide a platform for aspiring game providers resources to start their game designs</t>
   </si>
 </sst>
 </file>
@@ -525,8 +526,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="O16" sqref="O16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -538,7 +539,7 @@
     <col min="5" max="5" width="16" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="18.453125" customWidth="1"/>
     <col min="7" max="7" width="23.453125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="22.7265625" customWidth="1"/>
+    <col min="8" max="8" width="23.1796875" customWidth="1"/>
     <col min="9" max="9" width="11" customWidth="1"/>
     <col min="10" max="10" width="9" customWidth="1"/>
   </cols>
@@ -580,7 +581,7 @@
         <v>3</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>12</v>
@@ -606,7 +607,7 @@
         <v>3</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>12</v>
@@ -632,7 +633,7 @@
         <v>5</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>12</v>
@@ -647,7 +648,7 @@
         <v>25</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>26</v>
+        <v>37</v>
       </c>
       <c r="I6" s="3" t="s">
         <v>21</v>
@@ -658,7 +659,7 @@
         <v>7</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>12</v>
@@ -670,10 +671,10 @@
         <v>14</v>
       </c>
       <c r="G7" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="H7" s="3" t="s">
         <v>27</v>
-      </c>
-      <c r="H7" s="3" t="s">
-        <v>28</v>
       </c>
       <c r="I7" s="3" t="s">
         <v>22</v>
@@ -685,7 +686,7 @@
         <v>7</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>17</v>
@@ -697,10 +698,10 @@
         <v>15</v>
       </c>
       <c r="G8" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="H8" s="3" t="s">
         <v>29</v>
-      </c>
-      <c r="H8" s="3" t="s">
-        <v>30</v>
       </c>
       <c r="I8" s="3" t="s">
         <v>22</v>
@@ -712,7 +713,7 @@
         <v>9</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>12</v>
@@ -724,10 +725,10 @@
         <v>18</v>
       </c>
       <c r="G9" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="H9" s="3" t="s">
         <v>31</v>
-      </c>
-      <c r="H9" s="3" t="s">
-        <v>32</v>
       </c>
       <c r="I9" s="3" t="s">
         <v>22</v>

</xml_diff>

<commit_message>
Supervisor Meeting Minutes 110218.docx
</commit_message>
<xml_diff>
--- a/Documents/Change Log.xlsx
+++ b/Documents/Change Log.xlsx
@@ -163,12 +163,18 @@
       <name val="Doodle"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -198,18 +204,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -524,10 +532,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I13"/>
+  <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="O16" sqref="O16"/>
+      <selection activeCell="O7" sqref="O7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -544,13 +552,23 @@
     <col min="10" max="10" width="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="I1" s="1"/>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="I2" s="1"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A2" s="5"/>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="6"/>
+      <c r="J2" s="5"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A3" s="5"/>
       <c r="B3" s="2" t="s">
         <v>0</v>
       </c>
@@ -575,8 +593,10 @@
       <c r="I3" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" ht="58" x14ac:dyDescent="0.35">
+      <c r="J3" s="5"/>
+    </row>
+    <row r="4" spans="1:10" ht="58" x14ac:dyDescent="0.35">
+      <c r="A4" s="5"/>
       <c r="B4" s="3">
         <v>3</v>
       </c>
@@ -601,8 +621,10 @@
       <c r="I4" s="3" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" ht="130.5" x14ac:dyDescent="0.35">
+      <c r="J4" s="5"/>
+    </row>
+    <row r="5" spans="1:10" ht="130.5" x14ac:dyDescent="0.35">
+      <c r="A5" s="5"/>
       <c r="B5" s="3">
         <v>3</v>
       </c>
@@ -627,8 +649,10 @@
       <c r="I5" s="3" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="J5" s="5"/>
+    </row>
+    <row r="6" spans="1:10" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A6" s="5"/>
       <c r="B6" s="3">
         <v>5</v>
       </c>
@@ -653,8 +677,10 @@
       <c r="I6" s="3" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="J6" s="5"/>
+    </row>
+    <row r="7" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A7" s="5"/>
       <c r="B7" s="3">
         <v>7</v>
       </c>
@@ -679,9 +705,10 @@
       <c r="I7" s="3" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A8" s="1"/>
+      <c r="J7" s="5"/>
+    </row>
+    <row r="8" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A8" s="6"/>
       <c r="B8" s="3">
         <v>7</v>
       </c>
@@ -706,9 +733,10 @@
       <c r="I8" s="3" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" ht="130.5" x14ac:dyDescent="0.35">
-      <c r="A9" s="1"/>
+      <c r="J8" s="5"/>
+    </row>
+    <row r="9" spans="1:10" ht="130.5" x14ac:dyDescent="0.35">
+      <c r="A9" s="6"/>
       <c r="B9" s="3">
         <v>9</v>
       </c>
@@ -733,19 +761,21 @@
       <c r="I9" s="3" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
-      <c r="H10" s="1"/>
-      <c r="I10" s="1"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J9" s="5"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A10" s="6"/>
+      <c r="B10" s="6"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="6"/>
+      <c r="I10" s="6"/>
+      <c r="J10" s="5"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
@@ -756,7 +786,7 @@
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
@@ -767,7 +797,7 @@
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>

</xml_diff>